<commit_message>
Refine CSS styling: enhanced typography, colors, glassmorphism, and interactions
- Improved typography hierarchy (better font weights, sizing, spacing)
- Refined color palette (deeper backgrounds, optimized accents)
- Enhanced glassmorphism effects (24px blur + saturation boost)
- Premium interactive states (smooth focus, hover, active)
- Smoother animations (cubic-bezier easing, gentler pulses)
- Expanded spacing system (added 2xl value)
- Added accessibility features (focus-visible, reduced motion)
- Consistent styling across index, result, and error pages
- CSS-only improvements, no functional changes
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satish.kumar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F91D68-F215-4F1D-A845-9E6F46CA6D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB7EFD4-5159-4064-B7F9-C2916202F701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2DD4007F-9242-4CC1-98AB-54419377444F}"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">database!$A$1:$D$53</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="83">
   <si>
     <t>SAP ID</t>
   </si>
@@ -104,9 +107,6 @@
     <t>Safety</t>
   </si>
   <si>
-    <t>Team 9</t>
-  </si>
-  <si>
     <t>Aswin R</t>
   </si>
   <si>
@@ -122,9 +122,6 @@
     <t>ChellaKumar</t>
   </si>
   <si>
-    <t>Team 10</t>
-  </si>
-  <si>
     <t>Esakkimuthu.V</t>
   </si>
   <si>
@@ -279,13 +276,25 @@
   </si>
   <si>
     <t>ITDX</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>Coordination</t>
+  </si>
+  <si>
+    <t>Iyyappan</t>
+  </si>
+  <si>
+    <t>Satish</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,17 +316,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -327,6 +325,27 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -369,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -377,33 +396,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,735 +752,768 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC766FF-2B3F-4F79-B8B2-2C502C15DD76}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="16" style="6" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="10">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
         <v>11014949</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>6</v>
+      <c r="D2" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
+      <c r="A3" s="5">
         <v>11003216</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="A4" s="5">
         <v>11012912</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
         <v>11003955</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
+      <c r="D5" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="A6" s="5">
         <v>10014760</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
         <v>10013170</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
         <v>11008290</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>11007882</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
-        <v>11007882</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>11003222</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>11005149</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>10011590</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>10015248</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
-        <v>11003222</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>11013495</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>10011170</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>11000060</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>11002897</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>11009227</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>11000231</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>11012647</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="3" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>10011185</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>11015479</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>11010023</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
+        <v>11015187</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
+        <v>10013293</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
+        <v>10014684</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
+        <v>11007880</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A28" s="6">
+        <v>11010592</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="5">
+        <v>11005972</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A30" s="6">
+        <v>11012184</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
+        <v>11002308</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A32" s="6">
+        <v>11014795</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
+        <v>10007715</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="6">
+        <v>10009358</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A35" s="6">
+        <v>11011784</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A36" s="6">
+        <v>11003027</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
-        <v>11005149</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="D36" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A37" s="6">
+        <v>11012186</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A38" s="6">
+        <v>98765432</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D38" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="6">
+        <v>10014110</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A40" s="6">
+        <v>11004590</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A41" s="6">
+        <v>11000027</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A42" s="6">
+        <v>10015088</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="6">
+        <v>10007774</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A44" s="6">
+        <v>11015326</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A45" s="6">
+        <v>11011526</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A46" s="6">
+        <v>11013027</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="6">
+        <v>10011459</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="6">
+        <v>10011608</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A49" s="6">
+        <v>11003795</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A50" s="6">
+        <v>11002632</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A51" s="6">
+        <v>11006294</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A52" s="6">
+        <v>11011906</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
-        <v>10011590</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="3" t="s">
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A53" s="6">
+        <v>10011376</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
-        <v>10015248</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
-        <v>11013495</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
-        <v>10011170</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
-        <v>11000060</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
-        <v>11009227</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
-        <v>11000231</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
-        <v>11012647</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
-        <v>10011185</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
-        <v>11015479</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
-        <v>11010023</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="10">
-        <v>11015187</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="10">
-        <v>10013293</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="10">
-        <v>10014684</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="10">
-        <v>11007880</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="10">
-        <v>11010592</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
-        <v>11005972</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="10">
-        <v>11012184</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="10">
-        <v>11002308</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="D53" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="10">
-        <v>11014795</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="9">
-        <v>10007715</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="10">
-        <v>10009358</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="10">
-        <v>11011784</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="10">
-        <v>11003027</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="10">
-        <v>11012186</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="10">
-        <v>10014110</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="10">
-        <v>11004590</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="10">
-        <v>11000027</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="10">
-        <v>10015088</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="10">
-        <v>10007774</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="10">
-        <v>11015326</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="10">
-        <v>11011526</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="10">
-        <v>11013027</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="10">
-        <v>10011459</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="10">
-        <v>10011608</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="10">
-        <v>11003795</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="10">
-        <v>11002632</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="10">
-        <v>11006294</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="10">
-        <v>11011906</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="10">
-        <v>10011376</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:D53" xr:uid="{CEC766FF-2B3F-4F79-B8B2-2C502C15DD76}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D53">
+      <sortCondition ref="B1:B53"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1480,15 +1527,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B905000DA869114D80FA2D694CF64348" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ee9a2a4b52bb13dbe8a6ff146437804d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5f0b4e6f-5c96-42b0-840b-7f197de008bd" xmlns:ns4="d3200435-a422-457a-954b-2398b1a76c3f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="82dc1ebde49e90ba7fae93caff414059" ns3:_="" ns4:_="">
     <xsd:import namespace="5f0b4e6f-5c96-42b0-840b-7f197de008bd"/>
@@ -1727,6 +1765,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC0282C5-D988-48C9-908D-E6DB9498F185}">
   <ds:schemaRefs>
@@ -1738,14 +1785,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EB8528E-1742-4322-A490-B18E6530D5B2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{471DCFFB-6046-417B-835E-749F8E81E8A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1762,4 +1801,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EB8528E-1742-4322-A490-B18E6530D5B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>